<commit_message>
added funtion and elevation notes
</commit_message>
<xml_diff>
--- a/_analysis/bluff-lake-model/_dat/AssortedElevationNotes.xlsx
+++ b/_analysis/bluff-lake-model/_dat/AssortedElevationNotes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victoria Starnes\Documents\MSU\Hydrology Packet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victoria Starnes\Documents\GitHub\Bluff-Lake-Project\_analysis\bluff-lake-model\_dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47746E6A-CD6E-48F3-A3CF-0D173C172B17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6063A5D-F484-451C-8201-CFDE0257DF50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B68D1944-6400-4269-9E0F-895BD774C2C5}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="9">
-        <v>68.397120000000001</v>
+        <v>68.597120000000004</v>
       </c>
       <c r="C14" s="9">
         <v>23</v>

</xml_diff>